<commit_message>
charts added openmp and cilk
</commit_message>
<xml_diff>
--- a/Laufzeiten OpenMP.xlsx
+++ b/Laufzeiten OpenMP.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="12">
   <si>
     <t>Laufzeiten OpenMP Quicksort</t>
   </si>
@@ -43,9 +43,6 @@
   <si>
     <t>Sequentielle
 Laufzeit</t>
-  </si>
-  <si>
-    <t>Speedup</t>
   </si>
   <si>
     <t>1 Mio - random Zahlen, Seed= 987654321</t>
@@ -428,7 +425,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -479,7 +476,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
@@ -536,12 +532,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-AT" sz="1800" b="0" i="0" baseline="0">
+              <a:rPr lang="de-AT" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>Speedup 10 million random integers</a:t>
             </a:r>
-            <a:endParaRPr lang="de-AT">
+            <a:endParaRPr lang="de-AT" sz="1400">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -1135,12 +1131,12 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="de-AT" sz="1800" b="0" i="0" baseline="0">
+              <a:rPr lang="de-AT" sz="1400" b="0" i="0" baseline="0">
                 <a:effectLst/>
               </a:rPr>
               <a:t>Speedup 1 million random integers</a:t>
             </a:r>
-            <a:endParaRPr lang="de-AT">
+            <a:endParaRPr lang="de-AT" sz="1400">
               <a:effectLst/>
             </a:endParaRPr>
           </a:p>
@@ -1150,8 +1146,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14298600174978127"/>
-          <c:y val="2.7777777777777776E-2"/>
+          <c:x val="0.23743044619422571"/>
+          <c:y val="3.7037037037037035E-2"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1707,6 +1703,1206 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-AT" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Speedup 1 million random integers</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-AT" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$C$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speedup Implementation 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$38:$A$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$C$38:$C$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.0059729270092734</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.71546964207934605</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.81321004041333811</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58643044198599747</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.2878235480356876</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.23396223196647292</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.23924616537195911</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25189853076216712</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23881034244855084</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D657-440A-9154-70FC308CFE60}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$E$37</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speedup Implementation 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$38:$A$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$E$38:$E$46</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.82389318003830869</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77004970054753408</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.75798992128377563</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.58089807932575221</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.27608193967647232</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.24520208216293232</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.24089405245675624</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.25043421500090152</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.23561436520344706</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D657-440A-9154-70FC308CFE60}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1433609984"/>
+        <c:axId val="1433608736"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1433609984"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1433608736"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1433608736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Speedup</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1433609984"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="de-DE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="de-AT" sz="1400" b="0" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Speedup 10 million random integers</a:t>
+            </a:r>
+            <a:endParaRPr lang="de-AT" sz="1400">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$E$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speedup Implementation 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$52:$A$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$E$52:$E$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.77523802756229965</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.95202895449510594</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88314042738923526</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.67671924520590776</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.29612366759894349</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.27284087560997505</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.27077164107818075</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26944772492379798</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.25974859573447751</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2A1D-4FBA-A0A8-14BE9C9F1638}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$C$51</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speedup Implementation 1</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Tabelle1!$A$52:$A$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>48</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$C$52:$C$60</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1.0046153366389123</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1486977549198114</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.89739649111906994</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.68243424707906974</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.28575890293518613</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.26925326483091533</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.27169835398592135</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.26831479896378296</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.26728459013972239</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-2A1D-4FBA-A0A8-14BE9C9F1638}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1520672864"/>
+        <c:axId val="1520679520"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1520672864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Threads</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1520679520"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1520679520"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.2"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="de-AT"/>
+                  <a:t>Speedup</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="de-DE"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="de-DE"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1520672864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="de-DE"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="de-DE"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1787,6 +2983,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -2304,6 +3580,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2824,15 +5132,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>21647</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>13854</xdr:rowOff>
+      <xdr:colOff>12988</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>178376</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>21647</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>20781</xdr:rowOff>
+      <xdr:colOff>12988</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>185303</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2856,13 +5164,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>757670</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>31173</xdr:rowOff>
+      <xdr:rowOff>5195</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>757670</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>12122</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2876,6 +5184,66 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>12988</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>238991</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>12988</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>3463</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="8" name="Diagramm 7"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>4329</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>195694</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>4329</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>12122</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Diagramm 8"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -3150,11 +5518,13 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="18.42578125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3175,7 +5545,7 @@
     </row>
     <row r="4" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="20"/>
@@ -3205,13 +5575,13 @@
         <v>1</v>
       </c>
       <c r="C6" s="23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F6" s="16"/>
     </row>
@@ -3222,14 +5592,14 @@
       <c r="B7" s="13">
         <v>0.12209200000000001</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="25">
         <f>$F$16/B7</f>
         <v>1.005762503321721</v>
       </c>
       <c r="D7" s="13">
         <v>0.14593999999999999</v>
       </c>
-      <c r="E7" s="25">
+      <c r="E7" s="24">
         <f>$F$16/D7</f>
         <v>0.84141123444946953</v>
       </c>
@@ -3244,14 +5614,14 @@
       <c r="B8" s="1">
         <v>0.12733800000000001</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="25">
         <f t="shared" ref="C8:C15" si="0">$F$16/B8</f>
         <v>0.9643276598937911</v>
       </c>
       <c r="D8" s="1">
         <v>0.121333</v>
       </c>
-      <c r="E8" s="25">
+      <c r="E8" s="24">
         <f t="shared" ref="E8:E15" si="1">$F$16/D8</f>
         <v>1.0120540624195855</v>
       </c>
@@ -3266,14 +5636,14 @@
       <c r="B9" s="1">
         <v>0.12584300000000001</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="25">
         <f t="shared" si="0"/>
         <v>0.97578375877526413</v>
       </c>
       <c r="D9" s="1">
         <v>0.15187200000000001</v>
       </c>
-      <c r="E9" s="25">
+      <c r="E9" s="24">
         <f t="shared" si="1"/>
         <v>0.80854637823664377</v>
       </c>
@@ -3288,14 +5658,14 @@
       <c r="B10" s="1">
         <v>0.124541</v>
       </c>
-      <c r="C10" s="26">
+      <c r="C10" s="25">
         <f t="shared" si="0"/>
         <v>0.98598498129576262</v>
       </c>
       <c r="D10" s="1">
         <v>0.128164</v>
       </c>
-      <c r="E10" s="25">
+      <c r="E10" s="24">
         <f t="shared" si="1"/>
         <v>0.95811269588617376</v>
       </c>
@@ -3310,14 +5680,14 @@
       <c r="B11" s="1">
         <v>0.13614799999999999</v>
       </c>
-      <c r="C11" s="26">
+      <c r="C11" s="25">
         <f t="shared" si="0"/>
         <v>0.90192698795102078</v>
       </c>
       <c r="D11" s="1">
         <v>0.12925300000000001</v>
       </c>
-      <c r="E11" s="25">
+      <c r="E11" s="24">
         <f t="shared" si="1"/>
         <v>0.95004027415654235</v>
       </c>
@@ -3332,14 +5702,14 @@
       <c r="B12" s="1">
         <v>0.13092000000000001</v>
       </c>
-      <c r="C12" s="26">
+      <c r="C12" s="25">
         <f t="shared" si="0"/>
         <v>0.93794344298468968</v>
       </c>
       <c r="D12" s="1">
         <v>0.18146200000000001</v>
       </c>
-      <c r="E12" s="25">
+      <c r="E12" s="24">
         <f t="shared" si="1"/>
         <v>0.67670121323227761</v>
       </c>
@@ -3354,14 +5724,14 @@
       <c r="B13" s="1">
         <v>0.14111099999999999</v>
       </c>
-      <c r="C13" s="26">
+      <c r="C13" s="25">
         <f t="shared" si="0"/>
         <v>0.87020540961055892</v>
       </c>
       <c r="D13" s="22">
         <v>0.16760700000000001</v>
       </c>
-      <c r="E13" s="25">
+      <c r="E13" s="24">
         <f>$F$16/D13</f>
         <v>0.73263977969628702</v>
       </c>
@@ -3376,14 +5746,14 @@
       <c r="B14" s="1">
         <v>0.12114999999999999</v>
       </c>
-      <c r="C14" s="26">
+      <c r="C14" s="25">
         <f t="shared" si="0"/>
         <v>1.0135827945155227</v>
       </c>
       <c r="D14" s="1">
         <v>0.172818</v>
       </c>
-      <c r="E14" s="25">
+      <c r="E14" s="24">
         <f>$F$16/D14</f>
         <v>0.71054841252390133</v>
       </c>
@@ -3398,14 +5768,14 @@
       <c r="B15" s="11">
         <v>0.15071699999999999</v>
       </c>
-      <c r="C15" s="27">
+      <c r="C15" s="26">
         <f t="shared" si="0"/>
         <v>0.81474256756408092</v>
       </c>
       <c r="D15" s="11">
         <v>0.17877399999999999</v>
       </c>
-      <c r="E15" s="28">
+      <c r="E15" s="27">
         <f t="shared" si="1"/>
         <v>0.68687591906851997</v>
       </c>
@@ -3421,7 +5791,7 @@
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" s="20"/>
       <c r="C18" s="20"/>
@@ -3451,13 +5821,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="23" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>1</v>
       </c>
       <c r="E20" s="23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F20" s="16"/>
     </row>
@@ -3468,14 +5838,14 @@
       <c r="B21" s="13">
         <v>1.4973240000000001</v>
       </c>
-      <c r="C21" s="26">
+      <c r="C21" s="25">
         <f>$F$30/B21</f>
         <v>0.90879313881149149</v>
       </c>
       <c r="D21" s="13">
         <v>2.1056159999999999</v>
       </c>
-      <c r="E21" s="25">
+      <c r="E21" s="24">
         <f>$F$30/D21</f>
         <v>0.64625163267080876</v>
       </c>
@@ -3490,14 +5860,14 @@
       <c r="B22" s="1">
         <v>1.3441989999999999</v>
       </c>
-      <c r="C22" s="26">
+      <c r="C22" s="25">
         <f t="shared" ref="C22:C29" si="2">$F$30/B22</f>
         <v>1.0123186952064225</v>
       </c>
       <c r="D22" s="1">
         <v>1.870441</v>
       </c>
-      <c r="E22" s="25">
+      <c r="E22" s="24">
         <f t="shared" ref="E22:E29" si="3">$F$30/D22</f>
         <v>0.72750638901616127</v>
       </c>
@@ -3512,14 +5882,14 @@
       <c r="B23" s="1">
         <v>1.303037</v>
       </c>
-      <c r="C23" s="26">
+      <c r="C23" s="25">
         <f t="shared" si="2"/>
         <v>1.0442971134187116</v>
       </c>
       <c r="D23" s="1">
         <v>2.0303010000000001</v>
       </c>
-      <c r="E23" s="25">
+      <c r="E23" s="24">
         <f t="shared" si="3"/>
         <v>0.67022465032415279</v>
       </c>
@@ -3534,14 +5904,14 @@
       <c r="B24" s="1">
         <v>1.3168960000000001</v>
       </c>
-      <c r="C24" s="26">
+      <c r="C24" s="25">
         <f t="shared" si="2"/>
         <v>1.0333069413057505</v>
       </c>
       <c r="D24" s="1">
         <v>1.988702</v>
       </c>
-      <c r="E24" s="25">
+      <c r="E24" s="24">
         <f t="shared" si="3"/>
         <v>0.68424418428592004</v>
       </c>
@@ -3556,14 +5926,14 @@
       <c r="B25" s="1">
         <v>1.308381</v>
       </c>
-      <c r="C25" s="26">
+      <c r="C25" s="25">
         <f t="shared" si="2"/>
         <v>1.0400317474632983</v>
       </c>
       <c r="D25" s="1">
         <v>1.7811300000000001</v>
       </c>
-      <c r="E25" s="25">
+      <c r="E25" s="24">
         <f t="shared" si="3"/>
         <v>0.76398565954072839</v>
       </c>
@@ -3578,14 +5948,14 @@
       <c r="B26" s="1">
         <v>1.300797</v>
       </c>
-      <c r="C26" s="26">
+      <c r="C26" s="25">
         <f t="shared" si="2"/>
         <v>1.0460954151783697</v>
       </c>
       <c r="D26" s="1">
         <v>1.6125039999999999</v>
       </c>
-      <c r="E26" s="25">
+      <c r="E26" s="24">
         <f t="shared" si="3"/>
         <v>0.84387869907781798</v>
       </c>
@@ -3600,14 +5970,14 @@
       <c r="B27" s="1">
         <v>1.3362989999999999</v>
       </c>
-      <c r="C27" s="26">
+      <c r="C27" s="25">
         <f t="shared" si="2"/>
         <v>1.0183033720580332</v>
       </c>
       <c r="D27" s="1">
         <v>1.9669639999999999</v>
       </c>
-      <c r="E27" s="25">
+      <c r="E27" s="24">
         <f t="shared" si="3"/>
         <v>0.69180614275491459</v>
       </c>
@@ -3622,14 +5992,14 @@
       <c r="B28" s="1">
         <v>1.301072</v>
       </c>
-      <c r="C28" s="26">
+      <c r="C28" s="25">
         <f t="shared" si="2"/>
         <v>1.0458743080919255</v>
       </c>
       <c r="D28" s="1">
         <v>1.681832</v>
       </c>
-      <c r="E28" s="25">
+      <c r="E28" s="24">
         <f t="shared" si="3"/>
         <v>0.80909257153971248</v>
       </c>
@@ -3644,14 +6014,14 @@
       <c r="B29" s="11">
         <v>1.328735</v>
       </c>
-      <c r="C29" s="27">
+      <c r="C29" s="26">
         <f t="shared" si="2"/>
         <v>1.02410019889427</v>
       </c>
       <c r="D29" s="11">
         <v>1.867248</v>
       </c>
-      <c r="E29" s="28">
+      <c r="E29" s="27">
         <f t="shared" si="3"/>
         <v>0.72875042724789518</v>
       </c>
@@ -3668,7 +6038,7 @@
     <row r="32" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="1:6" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -3682,7 +6052,7 @@
     </row>
     <row r="35" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B35" s="20"/>
       <c r="C35" s="20"/>
@@ -3706,19 +6076,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="14"/>
       <c r="B37" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="24" t="s">
-        <v>6</v>
+      <c r="C37" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E37" s="24" t="s">
-        <v>6</v>
+      <c r="E37" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="F37" s="16"/>
     </row>
@@ -3729,14 +6099,14 @@
       <c r="B38" s="13">
         <v>0.121195</v>
       </c>
-      <c r="C38" s="26">
+      <c r="C38" s="25">
         <f>$F$47/B38</f>
         <v>1.0059729270092734</v>
       </c>
       <c r="D38" s="13">
         <v>0.147979</v>
       </c>
-      <c r="E38" s="25">
+      <c r="E38" s="24">
         <f>$F$47/D38</f>
         <v>0.82389318003830869</v>
       </c>
@@ -3751,14 +6121,14 @@
       <c r="B39" s="1">
         <v>0.170404</v>
       </c>
-      <c r="C39" s="26">
+      <c r="C39" s="25">
         <f t="shared" ref="C39:C46" si="4">$F$47/B39</f>
         <v>0.71546964207934605</v>
       </c>
       <c r="D39" s="1">
         <v>0.15832599999999999</v>
       </c>
-      <c r="E39" s="25">
+      <c r="E39" s="24">
         <f t="shared" ref="E39:E46" si="5">$F$47/D39</f>
         <v>0.77004970054753408</v>
       </c>
@@ -3773,14 +6143,14 @@
       <c r="B40" s="1">
         <v>0.149923</v>
       </c>
-      <c r="C40" s="26">
+      <c r="C40" s="25">
         <f t="shared" si="4"/>
         <v>0.81321004041333811</v>
       </c>
       <c r="D40" s="1">
         <v>0.16084499999999999</v>
       </c>
-      <c r="E40" s="25">
+      <c r="E40" s="24">
         <f t="shared" si="5"/>
         <v>0.75798992128377563</v>
       </c>
@@ -3795,14 +6165,14 @@
       <c r="B41" s="1">
         <v>0.2079</v>
       </c>
-      <c r="C41" s="26">
+      <c r="C41" s="25">
         <f t="shared" si="4"/>
         <v>0.58643044198599747</v>
       </c>
       <c r="D41" s="1">
         <v>0.20988000000000001</v>
       </c>
-      <c r="E41" s="25">
+      <c r="E41" s="24">
         <f t="shared" si="5"/>
         <v>0.58089807932575221</v>
       </c>
@@ -3817,14 +6187,14 @@
       <c r="B42" s="1">
         <v>0.42358899999999999</v>
       </c>
-      <c r="C42" s="26">
+      <c r="C42" s="25">
         <f t="shared" si="4"/>
         <v>0.2878235480356876</v>
       </c>
       <c r="D42" s="1">
         <v>0.441604</v>
       </c>
-      <c r="E42" s="25">
+      <c r="E42" s="24">
         <f t="shared" si="5"/>
         <v>0.27608193967647232</v>
       </c>
@@ -3839,14 +6209,14 @@
       <c r="B43" s="1">
         <v>0.52110500000000004</v>
       </c>
-      <c r="C43" s="26">
+      <c r="C43" s="25">
         <f t="shared" si="4"/>
         <v>0.23396223196647292</v>
       </c>
       <c r="D43" s="1">
         <v>0.49721799999999999</v>
       </c>
-      <c r="E43" s="25">
+      <c r="E43" s="24">
         <f t="shared" si="5"/>
         <v>0.24520208216293232</v>
       </c>
@@ -3861,14 +6231,14 @@
       <c r="B44" s="1">
         <v>0.50959600000000005</v>
       </c>
-      <c r="C44" s="26">
+      <c r="C44" s="25">
         <f t="shared" si="4"/>
         <v>0.23924616537195911</v>
       </c>
       <c r="D44" s="22">
         <v>0.50610999999999995</v>
       </c>
-      <c r="E44" s="25">
+      <c r="E44" s="24">
         <f t="shared" si="5"/>
         <v>0.24089405245675624</v>
       </c>
@@ -3883,14 +6253,14 @@
       <c r="B45" s="1">
         <v>0.48399999999999999</v>
       </c>
-      <c r="C45" s="26">
+      <c r="C45" s="25">
         <f t="shared" si="4"/>
         <v>0.25189853076216712</v>
       </c>
       <c r="D45" s="1">
         <v>0.48682999999999998</v>
       </c>
-      <c r="E45" s="25">
+      <c r="E45" s="24">
         <f t="shared" si="5"/>
         <v>0.25043421500090152</v>
       </c>
@@ -3905,14 +6275,14 @@
       <c r="B46" s="11">
         <v>0.51052600000000004</v>
       </c>
-      <c r="C46" s="27">
+      <c r="C46" s="26">
         <f t="shared" si="4"/>
         <v>0.23881034244855084</v>
       </c>
       <c r="D46" s="11">
         <v>0.51745099999999999</v>
       </c>
-      <c r="E46" s="28">
+      <c r="E46" s="27">
         <f t="shared" si="5"/>
         <v>0.23561436520344706</v>
       </c>
@@ -3922,16 +6292,16 @@
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E47" t="s">
-        <v>10</v>
-      </c>
-      <c r="F47" s="29">
+        <v>9</v>
+      </c>
+      <c r="F47" s="28">
         <f>AVERAGE(F38:F46)</f>
         <v>0.12191888888888888</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="20" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B49" s="20"/>
       <c r="C49" s="20"/>
@@ -3955,19 +6325,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="14"/>
       <c r="B51" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C51" s="24" t="s">
-        <v>6</v>
+      <c r="C51" s="23" t="s">
+        <v>10</v>
       </c>
       <c r="D51" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E51" s="24" t="s">
-        <v>6</v>
+      <c r="E51" s="23" t="s">
+        <v>11</v>
       </c>
       <c r="F51" s="16"/>
     </row>
@@ -3978,14 +6348,14 @@
       <c r="B52" s="13">
         <v>1.3610660000000001</v>
       </c>
-      <c r="C52" s="26">
+      <c r="C52" s="25">
         <f>$F$61/B52</f>
         <v>1.0046153366389123</v>
       </c>
       <c r="D52" s="13">
         <v>1.7637780000000001</v>
       </c>
-      <c r="E52" s="25">
+      <c r="E52" s="24">
         <f>$F$61/D52</f>
         <v>0.77523802756229965</v>
       </c>
@@ -4000,14 +6370,14 @@
       <c r="B53" s="1">
         <v>1.1903459999999999</v>
       </c>
-      <c r="C53" s="26">
+      <c r="C53" s="25">
         <f t="shared" ref="C53:C60" si="6">$F$61/B53</f>
         <v>1.1486977549198114</v>
       </c>
       <c r="D53" s="1">
         <v>1.4362459999999999</v>
       </c>
-      <c r="E53" s="25">
+      <c r="E53" s="24">
         <f t="shared" ref="E53:E60" si="7">$F$61/D53</f>
         <v>0.95202895449510594</v>
       </c>
@@ -4022,14 +6392,14 @@
       <c r="B54" s="1">
         <v>1.5236829999999999</v>
       </c>
-      <c r="C54" s="26">
+      <c r="C54" s="25">
         <f t="shared" si="6"/>
         <v>0.89739649111906994</v>
       </c>
       <c r="D54" s="1">
         <v>1.548279</v>
       </c>
-      <c r="E54" s="25">
+      <c r="E54" s="24">
         <f t="shared" si="7"/>
         <v>0.88314042738923526</v>
       </c>
@@ -4044,14 +6414,14 @@
       <c r="B55" s="1">
         <v>2.0036330000000002</v>
       </c>
-      <c r="C55" s="26">
+      <c r="C55" s="25">
         <f t="shared" si="6"/>
         <v>0.68243424707906974</v>
       </c>
       <c r="D55" s="1">
         <v>2.0205540000000002</v>
       </c>
-      <c r="E55" s="25">
+      <c r="E55" s="24">
         <f t="shared" si="7"/>
         <v>0.67671924520590776</v>
       </c>
@@ -4066,14 +6436,14 @@
       <c r="B56" s="1">
         <v>4.7849700000000004</v>
       </c>
-      <c r="C56" s="26">
+      <c r="C56" s="25">
         <f t="shared" si="6"/>
         <v>0.28575890293518613</v>
       </c>
       <c r="D56" s="1">
         <v>4.617489</v>
       </c>
-      <c r="E56" s="25">
+      <c r="E56" s="24">
         <f t="shared" si="7"/>
         <v>0.29612366759894349</v>
       </c>
@@ -4088,14 +6458,14 @@
       <c r="B57" s="1">
         <v>5.0782959999999999</v>
       </c>
-      <c r="C57" s="26">
+      <c r="C57" s="25">
         <f t="shared" si="6"/>
         <v>0.26925326483091533</v>
       </c>
       <c r="D57" s="1">
         <v>5.0115210000000001</v>
       </c>
-      <c r="E57" s="25">
+      <c r="E57" s="24">
         <f t="shared" si="7"/>
         <v>0.27284087560997505</v>
       </c>
@@ -4110,14 +6480,14 @@
       <c r="B58" s="1">
         <v>5.0325949999999997</v>
       </c>
-      <c r="C58" s="26">
+      <c r="C58" s="25">
         <f t="shared" si="6"/>
         <v>0.27169835398592135</v>
       </c>
       <c r="D58" s="22">
         <v>5.0498190000000003</v>
       </c>
-      <c r="E58" s="25">
+      <c r="E58" s="24">
         <f t="shared" si="7"/>
         <v>0.27077164107818075</v>
       </c>
@@ -4132,14 +6502,14 @@
       <c r="B59" s="1">
         <v>5.0960580000000002</v>
       </c>
-      <c r="C59" s="26">
+      <c r="C59" s="25">
         <f t="shared" si="6"/>
         <v>0.26831479896378296</v>
       </c>
       <c r="D59" s="1">
         <v>5.0746310000000001</v>
       </c>
-      <c r="E59" s="25">
+      <c r="E59" s="24">
         <f t="shared" si="7"/>
         <v>0.26944772492379798</v>
       </c>
@@ -4154,14 +6524,14 @@
       <c r="B60" s="11">
         <v>5.1157000000000004</v>
       </c>
-      <c r="C60" s="27">
+      <c r="C60" s="26">
         <f t="shared" si="6"/>
         <v>0.26728459013972239</v>
       </c>
       <c r="D60" s="11">
         <v>5.2641200000000001</v>
       </c>
-      <c r="E60" s="28">
+      <c r="E60" s="27">
         <f t="shared" si="7"/>
         <v>0.25974859573447751</v>
       </c>
@@ -4171,9 +6541,9 @@
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
-        <v>10</v>
-      </c>
-      <c r="F61" s="29">
+        <v>9</v>
+      </c>
+      <c r="F61" s="28">
         <f>AVERAGE(F52:F60)</f>
         <v>1.3673477777777778</v>
       </c>

</xml_diff>